<commit_message>
add new database build daily get stock exe
</commit_message>
<xml_diff>
--- a/excel/tw_2317.xlsx
+++ b/excel/tw_2317.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2460" uniqueCount="2460">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2462" uniqueCount="2462">
   <si>
     <t>index</t>
   </si>
@@ -7394,6 +7394,12 @@
   </si>
   <si>
     <t>2020-01-20 00:00:00</t>
+  </si>
+  <si>
+    <t>2020-01-30 00:00:00</t>
+  </si>
+  <si>
+    <t>2020-01-31 00:00:00</t>
   </si>
 </sst>
 </file>
@@ -7751,7 +7757,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L2450"/>
+  <dimension ref="A1:L2452"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -100854,6 +100860,82 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2451" spans="1:12">
+      <c r="A2451" s="1">
+        <v>2449</v>
+      </c>
+      <c r="B2451" t="s">
+        <v>2460</v>
+      </c>
+      <c r="C2451">
+        <v>153655274</v>
+      </c>
+      <c r="D2451">
+        <v>12913538375</v>
+      </c>
+      <c r="E2451">
+        <v>85.5</v>
+      </c>
+      <c r="F2451">
+        <v>86.2</v>
+      </c>
+      <c r="G2451">
+        <v>83.09999999999999</v>
+      </c>
+      <c r="H2451">
+        <v>83.09999999999999</v>
+      </c>
+      <c r="I2451">
+        <v>-9.199999999999999</v>
+      </c>
+      <c r="J2451">
+        <v>63060</v>
+      </c>
+      <c r="K2451">
+        <v>2317</v>
+      </c>
+      <c r="L2451">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2452" spans="1:12">
+      <c r="A2452" s="1">
+        <v>2450</v>
+      </c>
+      <c r="B2452" t="s">
+        <v>2461</v>
+      </c>
+      <c r="C2452">
+        <v>69686948</v>
+      </c>
+      <c r="D2452">
+        <v>5823335061</v>
+      </c>
+      <c r="E2452">
+        <v>83</v>
+      </c>
+      <c r="F2452">
+        <v>84.90000000000001</v>
+      </c>
+      <c r="G2452">
+        <v>82.59999999999999</v>
+      </c>
+      <c r="H2452">
+        <v>83.2</v>
+      </c>
+      <c r="I2452">
+        <v>0.1</v>
+      </c>
+      <c r="J2452">
+        <v>28528</v>
+      </c>
+      <c r="K2452">
+        <v>2317</v>
+      </c>
+      <c r="L2452">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>